<commit_message>
Added and updated data files
</commit_message>
<xml_diff>
--- a/Script Package/data_files/Test_EPD_384_wp.xlsx
+++ b/Script Package/data_files/Test_EPD_384_wp.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuni.sharepoint.com/sites/TG-AntiviralsandEV-VLPs/Shared Documents/General/Manuscripts/Python assisted EV diagnostics/Data/Example files for GitHub/data_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fsheky\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{EEA4CFDC-F598-49FF-B027-8E505C0E3FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C575669-6CB8-486A-AC3C-F15190B2A5C7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02029A3-03D5-4236-984F-223934925CE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36870" yWindow="1515" windowWidth="34080" windowHeight="17160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30195" yWindow="2415" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="4" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="SCR_virus1_ANALYSIS" sheetId="2" r:id="rId3"/>
     <sheet name="SCR_virus1_CALC" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" iterateCount="1" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -620,12 +620,6 @@
     <t>PFU/ml</t>
   </si>
   <si>
-    <t>Test EPD file</t>
-  </si>
-  <si>
-    <t>Contains one 96-well plate of raw end-point dilution assay data quantifying CVB1 infectivity in GMK cells.</t>
-  </si>
-  <si>
     <t>- GMK cells</t>
   </si>
   <si>
@@ -656,12 +650,6 @@
     <t>- Run script by typing "python EPDScript_384.py"</t>
   </si>
   <si>
-    <t>- Select master file: example_master_file.xlsx</t>
-  </si>
-  <si>
-    <t>- Select data file: Test EPD.xlsx</t>
-  </si>
-  <si>
     <t>- Select data sheet: Test EPD</t>
   </si>
   <si>
@@ -695,13 +683,25 @@
     <t>- Dilution rate: 6 (i.e. 6-fold dilution series)</t>
   </si>
   <si>
-    <t>Results are found from the scripted data file and from master file.</t>
-  </si>
-  <si>
     <t>Alamar Blue</t>
   </si>
   <si>
     <t>Alamar Blue 384</t>
+  </si>
+  <si>
+    <t>Test EPD 384wp file</t>
+  </si>
+  <si>
+    <t>Contains one 96-well plate of raw end-point dilution assay data in 384-well plate quantifying CVB1 infectivity in GMK cells.</t>
+  </si>
+  <si>
+    <t>Results are found from the this scripted data file and from master file.</t>
+  </si>
+  <si>
+    <t>- Select master file: Example_master_file.xlsx</t>
+  </si>
+  <si>
+    <t>- Select data file: Test_EPD_384wp.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1119,135 +1119,135 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68FBCF9F-F43C-4FD8-AB45-F012CE1AFF95}">
   <dimension ref="B2:B32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
-        <v>194</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>195</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" s="10" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" s="9" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="16" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B16" s="10" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="10" t="s">
-        <v>206</v>
+        <v>220</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="10" t="s">
-        <v>207</v>
+        <v>221</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" s="10" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="10" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" s="10" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" s="10" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" s="10" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
@@ -1264,7 +1264,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y175"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E113" sqref="E113"/>
     </sheetView>
   </sheetViews>
@@ -1360,7 +1360,7 @@
         <v>1</v>
       </c>
       <c r="L3" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -1875,7 +1875,7 @@
         <v>50</v>
       </c>
       <c r="E31" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
@@ -1901,7 +1901,7 @@
         <v>54</v>
       </c>
       <c r="E38" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -2676,7 +2676,7 @@
         <v>114</v>
       </c>
       <c r="E112" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -3929,16 +3929,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="fa612793-f91f-4de3-98ba-0e3886ad2ae2" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c0336683-2dd7-41cc-81b9-e80359f27e17">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4154,22 +4150,22 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="fa612793-f91f-4de3-98ba-0e3886ad2ae2" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c0336683-2dd7-41cc-81b9-e80359f27e17">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F64EE739-68CE-42B1-867C-2C78C790A572}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9C3976A-E79D-48F3-9857-B877DF4AB0C0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="fa612793-f91f-4de3-98ba-0e3886ad2ae2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="c0336683-2dd7-41cc-81b9-e80359f27e17"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4195,9 +4191,13 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9C3976A-E79D-48F3-9857-B877DF4AB0C0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F64EE739-68CE-42B1-867C-2C78C790A572}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fa612793-f91f-4de3-98ba-0e3886ad2ae2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="c0336683-2dd7-41cc-81b9-e80359f27e17"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>